<commit_message>
Add deployment to github pages
</commit_message>
<xml_diff>
--- a/questions_and_answers.xlsx
+++ b/questions_and_answers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyubo/Projects/captain-test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyubo/Projects/captain-test/captain-test-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCF4EEB-7FA2-A941-ABFF-861448110AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8EEDD6-F490-8749-96C1-8454B6F69DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9050,11 +9050,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F776"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="74" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>